<commit_message>
submit : server Add
</commit_message>
<xml_diff>
--- a/ExcelConfig/items.xlsx
+++ b/ExcelConfig/items.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -199,12 +199,158 @@
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>智力之冠</t>
+  </si>
+  <si>
+    <t>勇士头盔</t>
+  </si>
+  <si>
+    <t>迅猛面罩</t>
+  </si>
+  <si>
+    <t>远行护腿</t>
+  </si>
+  <si>
+    <t>勇士战靴</t>
+  </si>
+  <si>
+    <t>迅猛便鞋</t>
+  </si>
+  <si>
+    <t>棉手套</t>
+  </si>
+  <si>
+    <t>铁护碗</t>
+  </si>
+  <si>
+    <t>迅猛手套</t>
+  </si>
+  <si>
+    <t>法术披风</t>
+  </si>
+  <si>
+    <t>勇士护甲</t>
+  </si>
+  <si>
+    <t>影子披风</t>
+  </si>
+  <si>
+    <t>学者之冠</t>
+  </si>
+  <si>
+    <t>寒铁头盔</t>
+  </si>
+  <si>
+    <t>敏捷面罩</t>
+  </si>
+  <si>
+    <t>飞行护腿</t>
+  </si>
+  <si>
+    <t>寒铁战靴</t>
+  </si>
+  <si>
+    <t>敏捷便鞋</t>
+  </si>
+  <si>
+    <t>学者长袍</t>
+  </si>
+  <si>
+    <t>寒铁护甲</t>
+  </si>
+  <si>
+    <t>敏捷披风</t>
+  </si>
+  <si>
+    <t>魔法手套</t>
+  </si>
+  <si>
+    <t>寒铁护碗</t>
+  </si>
+  <si>
+    <t>敏捷手套</t>
+  </si>
+  <si>
+    <t>圣者之冠</t>
+  </si>
+  <si>
+    <t>秘银头盔</t>
+  </si>
+  <si>
+    <t>神秘面罩</t>
+  </si>
+  <si>
+    <t>圣者护腿</t>
+  </si>
+  <si>
+    <t>秘银战靴</t>
+  </si>
+  <si>
+    <t>龙皮便鞋</t>
+  </si>
+  <si>
+    <t>圣者手套</t>
+  </si>
+  <si>
+    <t>秘银护碗</t>
+  </si>
+  <si>
+    <t>火龙手套</t>
+  </si>
+  <si>
+    <t>圣者披风</t>
+  </si>
+  <si>
+    <t>秘银战甲</t>
+  </si>
+  <si>
+    <t>龙鹰披风</t>
+  </si>
+  <si>
+    <t>上古之冠</t>
+  </si>
+  <si>
+    <t>上古战靴</t>
+  </si>
+  <si>
+    <t>上古披风</t>
+  </si>
+  <si>
+    <t>上古护碗</t>
+  </si>
+  <si>
+    <t>天神头盔</t>
+  </si>
+  <si>
+    <t>天神战靴</t>
+  </si>
+  <si>
+    <t>天神披风</t>
+  </si>
+  <si>
+    <t>天神护碗</t>
+  </si>
+  <si>
+    <t>吸血面罩</t>
+  </si>
+  <si>
+    <t>Quility</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>品质</t>
+    <rPh sb="0" eb="1">
+      <t>pin zhi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +390,19 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -265,12 +424,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -612,13 +774,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,15 +788,15 @@
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" style="2" customWidth="1"/>
     <col min="3" max="4" width="11.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="2"/>
+    <col min="5" max="6" width="13.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -651,22 +813,25 @@
         <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -683,22 +848,25 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -715,22 +883,25 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -743,14 +914,23 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>10</v>
+      </c>
       <c r="I4" s="2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -763,17 +943,1196 @@
       <c r="E5" s="2">
         <v>1</v>
       </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>10</v>
+      </c>
       <c r="I5" s="2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
         <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
+        <v>1001</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="2">
+        <v>1002</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="2">
+        <v>1003</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>3</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>1004</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2">
+        <v>100</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
+        <v>1005</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2">
+        <v>100</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
+        <v>1006</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2">
+        <v>100</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>6</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
+        <v>1007</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="2">
+        <v>100</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>7</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="2">
+        <v>1008</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2">
+        <v>100</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>8</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="2">
+        <v>1009</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2">
+        <v>100</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>9</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="2">
+        <v>1010</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2">
+        <v>100</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>10</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="2">
+        <v>1011</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2">
+        <v>100</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>11</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="2">
+        <v>1012</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2">
+        <v>100</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>12</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="2">
+        <v>1013</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2">
+        <v>200</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>13</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="2">
+        <v>1014</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2">
+        <v>200</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>14</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="2">
+        <v>1015</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="2">
+        <v>200</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>15</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="2">
+        <v>1016</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2">
+        <v>200</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
+      <c r="H21" s="2">
+        <v>16</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="2">
+        <v>1017</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2">
+        <v>200</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+      <c r="H22" s="2">
+        <v>17</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="2">
+        <v>1018</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="2">
+        <v>200</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="H23" s="2">
+        <v>18</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="2">
+        <v>1019</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="2">
+        <v>200</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2</v>
+      </c>
+      <c r="H24" s="2">
+        <v>19</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="2">
+        <v>1020</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="2">
+        <v>200</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>20</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="2">
+        <v>1021</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="2">
+        <v>200</v>
+      </c>
+      <c r="E26" s="2">
+        <v>3</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
+      <c r="H26" s="2">
+        <v>21</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="2">
+        <v>1022</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="2">
+        <v>200</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2">
+        <v>22</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="2">
+        <v>1023</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="2">
+        <v>200</v>
+      </c>
+      <c r="E28" s="2">
+        <v>3</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2</v>
+      </c>
+      <c r="H28" s="2">
+        <v>23</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="2">
+        <v>1024</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="2">
+        <v>200</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2</v>
+      </c>
+      <c r="H29" s="2">
+        <v>24</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="2">
+        <v>1025</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="2">
+        <v>500</v>
+      </c>
+      <c r="E30" s="2">
+        <v>3</v>
+      </c>
+      <c r="F30" s="2">
+        <v>3</v>
+      </c>
+      <c r="H30" s="2">
+        <v>25</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="2">
+        <v>1026</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="2">
+        <v>500</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3</v>
+      </c>
+      <c r="F31" s="2">
+        <v>3</v>
+      </c>
+      <c r="H31" s="2">
+        <v>26</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="2">
+        <v>1027</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="2">
+        <v>500</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3</v>
+      </c>
+      <c r="H32" s="2">
+        <v>27</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="2">
+        <v>1028</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="2">
+        <v>500</v>
+      </c>
+      <c r="E33" s="2">
+        <v>3</v>
+      </c>
+      <c r="F33" s="2">
+        <v>3</v>
+      </c>
+      <c r="H33" s="2">
+        <v>28</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="2">
+        <v>1029</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="2">
+        <v>500</v>
+      </c>
+      <c r="E34" s="2">
+        <v>3</v>
+      </c>
+      <c r="F34" s="2">
+        <v>3</v>
+      </c>
+      <c r="H34" s="2">
+        <v>29</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="2">
+        <v>1030</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="2">
+        <v>500</v>
+      </c>
+      <c r="E35" s="2">
+        <v>3</v>
+      </c>
+      <c r="F35" s="2">
+        <v>3</v>
+      </c>
+      <c r="H35" s="2">
+        <v>30</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B36" s="2">
+        <v>1031</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="2">
+        <v>500</v>
+      </c>
+      <c r="E36" s="2">
+        <v>3</v>
+      </c>
+      <c r="F36" s="2">
+        <v>3</v>
+      </c>
+      <c r="H36" s="2">
+        <v>31</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" s="2">
+        <v>1032</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="2">
+        <v>500</v>
+      </c>
+      <c r="E37" s="2">
+        <v>3</v>
+      </c>
+      <c r="F37" s="2">
+        <v>3</v>
+      </c>
+      <c r="H37" s="2">
+        <v>32</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="2">
+        <v>1033</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="2">
+        <v>500</v>
+      </c>
+      <c r="E38" s="2">
+        <v>3</v>
+      </c>
+      <c r="F38" s="2">
+        <v>3</v>
+      </c>
+      <c r="H38" s="2">
+        <v>33</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="2">
+        <v>1034</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="2">
+        <v>500</v>
+      </c>
+      <c r="E39" s="2">
+        <v>3</v>
+      </c>
+      <c r="F39" s="2">
+        <v>3</v>
+      </c>
+      <c r="H39" s="2">
+        <v>34</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B40" s="2">
+        <v>1035</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="2">
+        <v>500</v>
+      </c>
+      <c r="E40" s="2">
+        <v>3</v>
+      </c>
+      <c r="F40" s="2">
+        <v>3</v>
+      </c>
+      <c r="H40" s="2">
+        <v>35</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B41" s="2">
+        <v>1036</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="2">
+        <v>500</v>
+      </c>
+      <c r="E41" s="2">
+        <v>3</v>
+      </c>
+      <c r="F41" s="2">
+        <v>3</v>
+      </c>
+      <c r="H41" s="2">
+        <v>36</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B42" s="2">
+        <v>1037</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3</v>
+      </c>
+      <c r="F42" s="2">
+        <v>4</v>
+      </c>
+      <c r="H42" s="2">
+        <v>37</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0</v>
+      </c>
+      <c r="K42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B43" s="2">
+        <v>1038</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E43" s="2">
+        <v>3</v>
+      </c>
+      <c r="F43" s="2">
+        <v>4</v>
+      </c>
+      <c r="H43" s="2">
+        <v>38</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0</v>
+      </c>
+      <c r="K43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B44" s="2">
+        <v>1039</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E44" s="2">
+        <v>3</v>
+      </c>
+      <c r="F44" s="2">
+        <v>4</v>
+      </c>
+      <c r="H44" s="2">
+        <v>39</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B45" s="2">
+        <v>1040</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E45" s="2">
+        <v>3</v>
+      </c>
+      <c r="F45" s="2">
+        <v>4</v>
+      </c>
+      <c r="H45" s="2">
+        <v>40</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B46" s="2">
+        <v>1041</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E46" s="2">
+        <v>3</v>
+      </c>
+      <c r="F46" s="2">
+        <v>5</v>
+      </c>
+      <c r="H46" s="2">
+        <v>41</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0</v>
+      </c>
+      <c r="K46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B47" s="2">
+        <v>1042</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3</v>
+      </c>
+      <c r="F47" s="2">
+        <v>5</v>
+      </c>
+      <c r="H47" s="2">
+        <v>42</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0</v>
+      </c>
+      <c r="K47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B48" s="2">
+        <v>1043</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E48" s="2">
+        <v>3</v>
+      </c>
+      <c r="F48" s="2">
+        <v>5</v>
+      </c>
+      <c r="H48" s="2">
+        <v>43</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B49" s="2">
+        <v>1044</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E49" s="2">
+        <v>3</v>
+      </c>
+      <c r="F49" s="2">
+        <v>5</v>
+      </c>
+      <c r="H49" s="2">
+        <v>44</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0</v>
+      </c>
+      <c r="K49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B50" s="2">
+        <v>1045</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E50" s="2">
+        <v>3</v>
+      </c>
+      <c r="F50" s="2">
+        <v>5</v>
+      </c>
+      <c r="H50" s="2">
+        <v>45</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0</v>
+      </c>
+      <c r="K50" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:T2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:U2">
       <formula1>"String,Int,DateTime,Float"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add pack sale item
</commit_message>
<xml_diff>
--- a/ExcelConfig/items.xlsx
+++ b/ExcelConfig/items.xlsx
@@ -1679,10 +1679,10 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1843,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="2">
-        <v>99</v>
+        <v>999</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1875,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="L5" s="2">
-        <v>99</v>
+        <v>999</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>